<commit_message>
WIND TURBINE DATA UPDATE AGAIN
Fuck me the wind turbine diameter should be 200m and hub height of 182.5. Values updated again...
</commit_message>
<xml_diff>
--- a/wind_turbine_11MW.xlsx
+++ b/wind_turbine_11MW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jc17718\Documents\GitHub\wind_turbine_ATMD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE2216E-E6F9-4454-99D1-17638D71CF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C5FF3B-AFC1-4562-928A-804B0DDD4BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -590,7 +590,8 @@
         <v>2</v>
       </c>
       <c r="B6" s="3">
-        <v>372</v>
+        <f>372+33</f>
+        <v>405</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -598,7 +599,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="3">
-        <v>167</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -606,7 +607,8 @@
         <v>7</v>
       </c>
       <c r="B8" s="4">
-        <v>206</v>
+        <f>365/2</f>
+        <v>182.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>